<commit_message>
Added gift card test case
</commit_message>
<xml_diff>
--- a/src/test/java/org/excel/Hackathonexcel.xlsx
+++ b/src/test/java/org/excel/Hackathonexcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2457210\IdeaProjects\Selenium\Hackathon\src\main\java\org\mp\constants\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2457257\IdeaProjects\Hackathon-project-cts\src\test\java\org\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C11C0F8-6B38-4832-BF2D-E753BCBF1431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3063F6F7-4D3A-47D0-BA37-AD40375C4C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{1D3BA2BF-7712-48BC-A655-4B9F16D3277F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{1D3BA2BF-7712-48BC-A655-4B9F16D3277F}"/>
   </bookViews>
   <sheets>
     <sheet name="Search Item" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Search Item</t>
   </si>
@@ -46,33 +46,12 @@
     <t>bookshelves</t>
   </si>
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
     <t>Sai</t>
   </si>
   <si>
     <t>Swapna</t>
   </si>
   <si>
-    <t>kattasaiswapna1@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Name </t>
-  </si>
-  <si>
-    <t>Message</t>
-  </si>
-  <si>
     <t>Hema</t>
   </si>
   <si>
@@ -85,7 +64,31 @@
     <t>Have a great day dear</t>
   </si>
   <si>
-    <t>63040626asdf</t>
+    <t>kattasaiswapna1@</t>
+  </si>
+  <si>
+    <t>receiverFirst Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">receiverLast Name </t>
+  </si>
+  <si>
+    <t>receiverEmail</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>senderFirst Name</t>
+  </si>
+  <si>
+    <t>senderLast Name</t>
+  </si>
+  <si>
+    <t>senderEmail</t>
+  </si>
+  <si>
+    <t>senderMobile</t>
   </si>
 </sst>
 </file>
@@ -507,44 +510,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A37A3E48-1AD5-4357-8B83-F8AE7C3DBC10}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="27.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
+      <c r="D2">
+        <v>6304062678</v>
       </c>
     </row>
   </sheetData>
@@ -559,43 +562,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63BCE884-C9D1-4E10-9C8C-109903FC2BF0}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working gift card testcase
</commit_message>
<xml_diff>
--- a/src/test/java/org/excel/Hackathonexcel.xlsx
+++ b/src/test/java/org/excel/Hackathonexcel.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2457257\IdeaProjects\Hackathon-project-cts\src\test\java\org\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3063F6F7-4D3A-47D0-BA37-AD40375C4C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF6CBC8-A62A-427C-8601-CE720CFD9EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{1D3BA2BF-7712-48BC-A655-4B9F16D3277F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{1D3BA2BF-7712-48BC-A655-4B9F16D3277F}"/>
   </bookViews>
   <sheets>
     <sheet name="Search Item" sheetId="1" r:id="rId1"/>
     <sheet name="Sender Details" sheetId="2" r:id="rId2"/>
     <sheet name="Receiver Details" sheetId="3" r:id="rId3"/>
+    <sheet name="Denomination" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Search Item</t>
   </si>
@@ -89,13 +90,25 @@
   </si>
   <si>
     <t>senderMobile</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +132,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -128,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -136,15 +154,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -562,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63BCE884-C9D1-4E10-9C8C-109903FC2BF0}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -607,4 +644,35 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F87E067E-CF8C-4728-BF0D-F1294E76327C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>